<commit_message>
Updated interface coverage and added even more TODOs
</commit_message>
<xml_diff>
--- a/StructureInterfaceCoverage.xlsx
+++ b/StructureInterfaceCoverage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{187BC8AF-116E-9F42-B323-B0EF40DA88FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94220CA-36E7-7847-9C7A-8E8F2219BB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="4240" windowWidth="38400" windowHeight="10660" xr2:uid="{4C3D585B-458E-5D4F-9908-4968E91B5E86}"/>
+    <workbookView xWindow="25600" yWindow="3480" windowWidth="24000" windowHeight="11420" xr2:uid="{4C3D585B-458E-5D4F-9908-4968E91B5E86}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="25">
   <si>
     <t>Structure</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>TODO</t>
+  </si>
+  <si>
+    <t>ThreeDVector</t>
   </si>
 </sst>
 </file>
@@ -174,20 +177,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -203,7 +206,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -499,13 +502,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA82DFC-6EF9-D243-AB9B-D0F30ADFAA9F}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,21 +527,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
       <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
@@ -588,37 +591,37 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -626,13 +629,13 @@
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -640,37 +643,37 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -678,28 +681,28 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -707,28 +710,28 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -736,13 +739,13 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -750,37 +753,37 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -788,37 +791,37 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -826,19 +829,19 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -846,37 +849,72 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement ICloneable on LinearRegressionResult
</commit_message>
<xml_diff>
--- a/StructureInterfaceCoverage.xlsx
+++ b/StructureInterfaceCoverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94220CA-36E7-7847-9C7A-8E8F2219BB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F67526-43D8-FC4E-B3BE-CCF05A53CDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="3480" windowWidth="24000" windowHeight="11420" xr2:uid="{4C3D585B-458E-5D4F-9908-4968E91B5E86}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24000" windowHeight="16000" xr2:uid="{4C3D585B-458E-5D4F-9908-4968E91B5E86}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -504,11 +504,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA82DFC-6EF9-D243-AB9B-D0F30ADFAA9F}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,8 +684,8 @@
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>23</v>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>21</v>
@@ -713,8 +713,8 @@
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>23</v>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Implemented IEquatable<IConvertible> in Exp
</commit_message>
<xml_diff>
--- a/StructureInterfaceCoverage.xlsx
+++ b/StructureInterfaceCoverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F67526-43D8-FC4E-B3BE-CCF05A53CDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30154ABF-62F9-3C44-BFF1-DA6ED1FF1C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24000" windowHeight="16000" xr2:uid="{4C3D585B-458E-5D4F-9908-4968E91B5E86}"/>
   </bookViews>
@@ -508,7 +508,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,8 +649,8 @@
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>23</v>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Implement IComparable on Exp
</commit_message>
<xml_diff>
--- a/StructureInterfaceCoverage.xlsx
+++ b/StructureInterfaceCoverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30154ABF-62F9-3C44-BFF1-DA6ED1FF1C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2473266-40BB-AD41-A42A-391D085C2DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24000" windowHeight="16000" xr2:uid="{4C3D585B-458E-5D4F-9908-4968E91B5E86}"/>
   </bookViews>
@@ -508,7 +508,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,20 +658,20 @@
       <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>23</v>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>23</v>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>23</v>
+      <c r="K5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Updated structure interface coverage spreadsheet
</commit_message>
<xml_diff>
--- a/StructureInterfaceCoverage.xlsx
+++ b/StructureInterfaceCoverage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2473266-40BB-AD41-A42A-391D085C2DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E08435-BAE1-884C-A701-B4D16F64ECEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24000" windowHeight="16000" xr2:uid="{4C3D585B-458E-5D4F-9908-4968E91B5E86}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22400" xr2:uid="{4C3D585B-458E-5D4F-9908-4968E91B5E86}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="26">
   <si>
     <t>Structure</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>ThreeDVector</t>
+  </si>
+  <si>
+    <t>AminoAcid</t>
   </si>
 </sst>
 </file>
@@ -206,9 +209,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -246,7 +249,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -352,7 +355,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -494,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -502,13 +505,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA82DFC-6EF9-D243-AB9B-D0F30ADFAA9F}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,7 +592,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -598,41 +601,65 @@
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
+      <c r="F3" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -641,36 +668,12 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -679,28 +682,37 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>14</v>
@@ -708,7 +720,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
@@ -737,13 +749,28 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>14</v>
@@ -751,37 +778,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="F9" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>14</v>
@@ -789,19 +792,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>23</v>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>14</v>
@@ -827,19 +830,37 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>14</v>
@@ -847,37 +868,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>14</v>
@@ -885,36 +888,74 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented ICloneable and a copy constructor to AminoAcid
</commit_message>
<xml_diff>
--- a/StructureInterfaceCoverage.xlsx
+++ b/StructureInterfaceCoverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E08435-BAE1-884C-A701-B4D16F64ECEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F767553-42B8-684C-9E5B-1CC4261367DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22400" xr2:uid="{4C3D585B-458E-5D4F-9908-4968E91B5E86}"/>
   </bookViews>
@@ -511,7 +511,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,8 +606,8 @@
       <c r="E3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>23</v>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>

</xml_diff>